<commit_message>
Gráficos por dia colocados em ordem pelo numero total de casos
</commit_message>
<xml_diff>
--- a/docs/Python/PA.xlsx
+++ b/docs/Python/PA.xlsx
@@ -1,101 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padulla\Documents\GitHub\corona_dash\docs\Python\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CB7E04-6A8F-4CE5-984B-DBD197259955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Clinico_total</t>
-  </si>
-  <si>
-    <t>Clinico_disp</t>
-  </si>
-  <si>
-    <t>uti_total</t>
-  </si>
-  <si>
-    <t>uti_disp</t>
-  </si>
-  <si>
-    <t>55.53%</t>
-  </si>
-  <si>
-    <t>91.15%</t>
-  </si>
-  <si>
-    <t>09/05/2020</t>
-  </si>
-  <si>
-    <t>55.18%</t>
-  </si>
-  <si>
-    <t>85.14%</t>
-  </si>
-  <si>
-    <t>10/05/2020</t>
-  </si>
-  <si>
-    <t>53.47%</t>
-  </si>
-  <si>
-    <t>82.63%</t>
-  </si>
-  <si>
-    <t>11/05/2020</t>
-  </si>
-  <si>
-    <t>55.78%</t>
-  </si>
-  <si>
-    <t>79.32%</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -114,23 +46,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -430,149 +353,210 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="12.140625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="12.28515625" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="8.5703125" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
+    <col width="8.7109375" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="8.140625" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Clinico_total</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Clinico_disp</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Clinico_disp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>uti_total</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>uti_disp</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>uti_disp</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>43959</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>1122</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>499</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>55.53%</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>192</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>91.15%</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>09/05/2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>1109</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>497</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>55.18%</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>249</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>85.14%</t>
+        </is>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>10/05/2020</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>1109</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>516</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>53.47%</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>259</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>45</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>82.63%</t>
+        </is>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>11/05/2020</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>1108</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>490</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>55.78%</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>266</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>55</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>79.32%</t>
+        </is>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J7" s="1"/>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12/05/2020</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1108</v>
+      </c>
+      <c r="C8" t="n">
+        <v>490</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>55.78%</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>266</v>
+      </c>
+      <c r="F8" t="n">
+        <v>55</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>79.32%</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>